<commit_message>
Corrected test_result, mapping rules
</commit_message>
<xml_diff>
--- a/mapping/mml_labtest_to_test_result.xlsx
+++ b/mapping/mml_labtest_to_test_result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="150">
   <si>
     <t>mmlLb:TestModule</t>
   </si>
@@ -60,9 +60,6 @@
     <t>mmlLb:statusCode</t>
   </si>
   <si>
-    <t>mmlLb0001</t>
-  </si>
-  <si>
     <t>mmlLb:statusCodeId</t>
   </si>
   <si>
@@ -365,66 +362,14 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[at0075]</t>
-  </si>
-  <si>
     <t>/context/other_context[at0001]/items[at0005]</t>
   </si>
   <si>
-    <t>＊現時点ではなし</t>
-    <rPh sb="1" eb="4">
-      <t>ゲンジテン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Facility']/items[at0001]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Department']/items[at0001]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Department']/items[at0011]</t>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Ward']/items[at0011]</t>
   </si>
   <si>
     <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Ward']/items[at0001]</t>
     <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[openEHR-EHR-CLUSTER.person_name.v1]/items[at0001]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[at0011]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Organisation']/items[at0001]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Organisation']/items[at0011]</t>
-  </si>
-  <si>
-    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Performed technician']/items[openEHR-EHR-CLUSTER.person_name.v1]/items[at0006]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0002]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.specimen.v1 and name/value='Specimen']/items[at0029]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.specimen.v1 and name/value='Specimen']/items[at0002]/items[at0001]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.specimen.v1 and name/value='Specimen']/items[at0039]/items[at0045]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0005]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0015]</t>
   </si>
   <si>
     <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0078 and name/value='Result']</t>
@@ -480,13 +425,146 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>☑</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[at0075]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mmlLb001</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>mid/final</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Facility']/items[at0001]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Facility']/items[at0011]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Department']/items[at0001]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Department']/items[at0011]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[openEHR-EHR-CLUSTER.person_name.v1]/items[at0001]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[at0011]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>☑</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Organisation']/items[at0001]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Organisation']/items[at0011]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Performed technician']/items[openEHR-EHR-CLUSTER.person_name.v1]/items[at0001]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Performed technician']/items[at0003]/items[at0011]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.free_text.v1 and name/value='Report memo']/items[at0001 and name/value='Free text']</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.specimen.v1 and name/value='Specimen']/items[at0029]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.specimen.v1 and name/value='Specimen']/items[at0002]/items[at0001]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0005]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0017]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.free_text.v1 and name/value='Lab test set']/items[at0001 and name/value='Free text']</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.specimen.v1 and name/value='Specimen']/items[at0039]/items[at0045]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0015]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0078 and name/value='Result']</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>繰り返しの範囲</t>
+    <rPh sb="0" eb="1">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カエ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ハンイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Memo、MemoFは該当するところに繰り返し</t>
+    <rPh sb="11" eb="13">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0057]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>up, down, normalはまとめてreference range guidance</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0005]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0057]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0002]</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -881,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="F47" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -906,10 +984,10 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="H1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -949,11 +1027,14 @@
         <v>5</v>
       </c>
       <c r="F4" s="2"/>
+      <c r="G4" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H4" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="81">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="40.5">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -966,8 +1047,11 @@
         <v>8</v>
       </c>
       <c r="F5" s="2"/>
+      <c r="G5" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="40.5">
@@ -983,11 +1067,14 @@
         <v>5</v>
       </c>
       <c r="F6" s="2"/>
+      <c r="G6" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H6" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="27">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -1000,12 +1087,15 @@
         <v>5</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="H7" t="s">
-        <v>114</v>
+      <c r="G7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="27">
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1018,11 +1108,14 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
+      <c r="G8" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="27">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -1035,15 +1128,18 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>14</v>
+        <v>121</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="27">
+    <row r="10" spans="1:11">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
@@ -1052,48 +1148,54 @@
         <v>5</v>
       </c>
       <c r="F10" s="2"/>
+      <c r="H10" s="4" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2"/>
+      <c r="G11" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H11" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="27">
+    <row r="12" spans="1:11">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>4</v>
@@ -1105,10 +1207,10 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -1116,15 +1218,18 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
+      <c r="G14" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="27">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>4</v>
@@ -1133,15 +1238,18 @@
         <v>5</v>
       </c>
       <c r="F15" s="2"/>
+      <c r="G15" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="27">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
@@ -1150,52 +1258,58 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17" s="2"/>
+      <c r="G17" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H17" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>30</v>
+      <c r="G18" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>4</v>
@@ -1207,28 +1321,31 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F20" s="2"/>
+      <c r="G20" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="H20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="27">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>4</v>
@@ -1237,17 +1354,20 @@
         <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="H21" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>4</v>
@@ -1259,28 +1379,31 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" s="2"/>
+      <c r="G23" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="27">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>4</v>
@@ -1289,17 +1412,20 @@
         <v>8</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="H24" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>4</v>
@@ -1311,10 +1437,10 @@
     </row>
     <row r="26" spans="1:8" ht="27">
       <c r="A26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
@@ -1322,15 +1448,18 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
+      <c r="G26" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="27">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>4</v>
@@ -1339,17 +1468,20 @@
         <v>5</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="H27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="27">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>4</v>
@@ -1361,28 +1493,31 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F29" s="2"/>
+      <c r="G29" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H29" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="27">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>4</v>
@@ -1391,14 +1526,20 @@
         <v>8</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>4</v>
@@ -1410,28 +1551,31 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F32" s="2"/>
+      <c r="G32" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H32" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>4</v>
@@ -1441,11 +1585,11 @@
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="27">
+    <row r="34" spans="1:8">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>4</v>
@@ -1454,14 +1598,14 @@
         <v>8</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>4</v>
@@ -1473,55 +1617,58 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F36" s="2"/>
+      <c r="G36" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H36" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="27">
+    <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
@@ -1529,15 +1676,18 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
+      <c r="G39" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H39" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="27">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>4</v>
@@ -1546,17 +1696,20 @@
         <v>5</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="H40" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="27">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>4</v>
@@ -1568,28 +1721,31 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F42" s="2"/>
+      <c r="G42" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H42" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>4</v>
@@ -1599,11 +1755,11 @@
       </c>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="27">
+    <row r="44" spans="1:8">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>4</v>
@@ -1612,14 +1768,14 @@
         <v>8</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>4</v>
@@ -1631,43 +1787,46 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F46" s="2"/>
+      <c r="G46" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H46" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
@@ -1675,15 +1834,18 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
+      <c r="G48" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H48" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="27">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>4</v>
@@ -1692,17 +1854,20 @@
         <v>5</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="H49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="27">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>4</v>
@@ -1716,23 +1881,23 @@
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>4</v>
@@ -1741,14 +1906,14 @@
         <v>8</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>4</v>
@@ -1757,14 +1922,14 @@
         <v>8</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>4</v>
@@ -1773,14 +1938,14 @@
         <v>8</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>4</v>
@@ -1789,15 +1954,15 @@
         <v>8</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
@@ -1805,68 +1970,80 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
+      <c r="G56" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H56" s="5" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F57" s="2"/>
+      <c r="G57" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H57" s="6" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="2"/>
+      <c r="G58" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H58" s="6" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F59" s="2"/>
-      <c r="H59" t="s">
-        <v>137</v>
+      <c r="G59" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>4</v>
@@ -1875,53 +2052,62 @@
         <v>8</v>
       </c>
       <c r="F60" s="2"/>
-      <c r="H60" t="s">
-        <v>137</v>
+      <c r="G60" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>93</v>
+      <c r="G61" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F62" s="2"/>
+      <c r="G62" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H62" s="7" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>4</v>
@@ -1930,17 +2116,20 @@
         <v>8</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>4</v>
@@ -1949,54 +2138,60 @@
         <v>8</v>
       </c>
       <c r="F64" s="2"/>
+      <c r="G64" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H64" s="6" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F66" s="2"/>
+      <c r="G66" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H66" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2004,7 +2199,7 @@
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>4</v>
@@ -2014,14 +2209,14 @@
       </c>
       <c r="F68" s="2"/>
       <c r="H68" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="27">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>4</v>
@@ -2030,14 +2225,14 @@
         <v>8</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>4</v>
@@ -2049,21 +2244,36 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F71" s="3"/>
       <c r="H71" t="s">
-        <v>127</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="H75" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="H76" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="H77" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated lab test module and mapping
</commit_message>
<xml_diff>
--- a/mapping/mml_labtest_to_test_result.xlsx
+++ b/mapping/mml_labtest_to_test_result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="190">
   <si>
     <t>mmlLb:TestModule</t>
   </si>
@@ -375,56 +375,6 @@
     <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0078 and name/value='Result']</t>
   </si>
   <si>
-    <t>また、数字の場合には単位もセットで記録されるようになっており、このあたりをひとまとめにしてResultに放り込む形です。</t>
-    <rPh sb="3" eb="5">
-      <t>スウジ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>タンイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>キロク</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>カタチ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>注）Laboratory testには ANY型が指定されており、数字や文字(コード）などの値を代入することができるようになっております。</t>
-    <rPh sb="0" eb="1">
-      <t>チュウ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>ガタ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>スウジ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>アタイ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ダイニュウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>☑</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -437,14 +387,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>mmlLb001</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>mid/final</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/protocol[at0004]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Professional Individual demographics']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation.v1 and name/value='Facility']/items[at0001]</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -482,10 +424,6 @@
   </si>
   <si>
     <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Performed technician']/items[openEHR-EHR-CLUSTER.person_name.v1]/items[at0001]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Performed technician']/items[at0003]/items[at0011]</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -595,6 +533,240 @@
   </si>
   <si>
     <t>context/Report ID</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.individual_professional.v1 and name/value='Performed technician']/items[at0003]/items[at0011]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-CLUSTER.individual_professional.v1</t>
+  </si>
+  <si>
+    <t>*1)mid/final</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*2)mmlLb001</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>また、数字の場合には単位もセットで記録されるようになっており、各データ型に対応した参照モデルの形でにしてResultに放り込む形です。</t>
+    <rPh sb="3" eb="5">
+      <t>スウジ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>タンイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>キロク</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ガタ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>タイオウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>カタチ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>カタチ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*1) mid, finalのいずれか</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*2) mmlLb0001と固定入力される（MML仕様の通り）</t>
+    <rPh sb="14" eb="16">
+      <t>コテイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>トオ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-CLUSTER.free_text.v1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Free text</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-CLUSTER.organisation.v1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Name of organisation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Identifier</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-CLUSTER.individual_professional.v1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-CLUSTER.person_name.v1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>unstructured name</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Professional identifier</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Name of organisation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Identifier</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-EVALUATION.clinical_synopsis.v1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Synopsis</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Specimen tissue type</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-OBSERVATION.lab_test.v1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Test name</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-CLUSTER.lab_result_annotation.v1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*3) Laboratory result identifier</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*3) DV_CODED_TEXTとして保存</t>
+    <rPh sb="20" eb="22">
+      <t>ホゾン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*4)Result</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*4)注）Laboratory testには ANY型が指定されており、数字や文字(コード）などの値を代入することができるようになっております。</t>
+    <rPh sb="3" eb="4">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ガタ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>スウジ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ダイニュウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reference range guidance</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>overall interpretation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*5)Reference range guidance</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*6)link to original lab test</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*5) 上限、下限、正常範囲内はテキストで保存</t>
+    <rPh sb="4" eb="6">
+      <t>ジョウゲン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>カゲン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>セイジョウ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>ハンイナイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ホゾン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*6) Multimedia?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Result comment</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -642,12 +814,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -664,7 +842,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -687,6 +865,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -990,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1015,7 +1202,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="H1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J1" t="s">
         <v>111</v>
@@ -1036,7 +1223,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1065,10 +1252,10 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>109</v>
@@ -1088,13 +1275,13 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>110</v>
@@ -1114,10 +1301,10 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>112</v>
@@ -1137,16 +1324,16 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1163,10 +1350,10 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J8" t="s">
         <v>113</v>
@@ -1185,11 +1372,11 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
-        <v>123</v>
+      <c r="J9" s="8" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1205,8 +1392,8 @@
         <v>5</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="J10" s="4" t="s">
-        <v>122</v>
+      <c r="J10" s="8" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1225,11 +1412,16 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="I11" s="4"/>
+        <v>117</v>
+      </c>
+      <c r="H11" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="J11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1262,7 +1454,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" ht="27">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1276,10 +1468,16 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="H14" t="s">
+        <v>162</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="J14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1296,10 +1494,13 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="J15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1318,7 +1519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" ht="27">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1334,10 +1535,16 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="H17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="J17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1356,10 +1563,13 @@
         <v>29</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="J18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1376,7 +1586,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" ht="27">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
@@ -1392,7 +1602,13 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="H20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="J20" t="s">
         <v>115</v>
@@ -1414,7 +1630,10 @@
         <v>19</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="J21" t="s">
         <v>114</v>
@@ -1450,13 +1669,19 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H23" t="s">
+        <v>166</v>
+      </c>
+      <c r="I23" t="s">
+        <v>167</v>
       </c>
       <c r="J23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="27">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -1472,10 +1697,16 @@
         <v>19</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H24" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="J24" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1506,10 +1737,16 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H26" t="s">
+        <v>162</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="J26" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1528,10 +1765,13 @@
         <v>19</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="J27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1564,10 +1804,16 @@
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H29" t="s">
+        <v>166</v>
+      </c>
+      <c r="I29" t="s">
+        <v>167</v>
       </c>
       <c r="J29" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="54">
@@ -1586,10 +1832,16 @@
         <v>19</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H30" t="s">
+        <v>154</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1622,10 +1874,16 @@
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H32" t="s">
+        <v>171</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="J32" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1688,10 +1946,10 @@
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J36" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1720,7 +1978,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" ht="27">
       <c r="A39" s="2" t="s">
         <v>60</v>
       </c>
@@ -1734,10 +1992,16 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H39" t="s">
+        <v>147</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="J39" t="s">
         <v>130</v>
-      </c>
-      <c r="J39" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1756,10 +2020,10 @@
         <v>19</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J40" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1792,10 +2056,13 @@
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="J42" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1858,10 +2125,13 @@
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="J46" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -1877,6 +2147,9 @@
         <v>57</v>
       </c>
       <c r="F47" s="2"/>
+      <c r="H47" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
@@ -1892,13 +2165,16 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="I48" t="s">
+        <v>177</v>
       </c>
       <c r="J48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="27">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
@@ -1914,10 +2190,16 @@
         <v>19</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H49" t="s">
+        <v>178</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="J49" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2028,10 +2310,16 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H56" t="s">
+        <v>176</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2050,13 +2338,13 @@
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" ht="27">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
@@ -2070,13 +2358,19 @@
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H58" t="s">
+        <v>178</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>185</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="27">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
@@ -2090,13 +2384,16 @@
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>183</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="27">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
@@ -2110,13 +2407,16 @@
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>183</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="27">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
@@ -2132,10 +2432,16 @@
         <v>92</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="H61" t="s">
+        <v>176</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2154,10 +2460,10 @@
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2176,10 +2482,7 @@
         <v>19</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2196,10 +2499,7 @@
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2230,10 +2530,13 @@
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="J66" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2266,10 +2569,16 @@
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="H68" t="s">
+        <v>178</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="J68" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2318,25 +2627,63 @@
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="J71" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="J75" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="J76" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="J77" t="s">
-        <v>146</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="J79" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="J80" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="10:10">
+      <c r="J81" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82" spans="10:10">
+      <c r="J82" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="83" spans="10:10">
+      <c r="J83" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="10:10">
+      <c r="J84" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="85" spans="10:10">
+      <c r="J85" s="9" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed value and units
</commit_message>
<xml_diff>
--- a/mapping/mml_labtest_to_test_result.xlsx
+++ b/mapping/mml_labtest_to_test_result.xlsx
@@ -868,10 +868,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0078 and name/value='Result']/unit</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0002]/value</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1069,10 +1065,16 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0007]</t>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0003]</t>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0003]/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1 and name/value='Laboratory result annotation']/items[at0007]/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-OBSERVATION.lab_test.v1 and name/value='Laboratory test']/data[at0001]/events[at0002 and name/value='Any event']/data[at0003]/items[at0078 and name/value='Result']/units</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -1526,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B75" workbookViewId="0">
-      <selection activeCell="K88" sqref="K88"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1736,7 +1738,7 @@
       </c>
       <c r="J9" s="4"/>
       <c r="K9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1756,7 +1758,7 @@
         <v>123</v>
       </c>
       <c r="K10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1770,7 +1772,7 @@
         <v>168</v>
       </c>
       <c r="K11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1818,7 +1820,7 @@
         <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1835,7 +1837,7 @@
       </c>
       <c r="F14" s="2"/>
       <c r="K14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1849,7 +1851,7 @@
         <v>168</v>
       </c>
       <c r="K15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1919,7 +1921,7 @@
         <v>25</v>
       </c>
       <c r="K18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1933,7 +1935,7 @@
         <v>168</v>
       </c>
       <c r="K19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="27">
@@ -1985,7 +1987,7 @@
         <v>131</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K21" t="s">
         <v>173</v>
@@ -2005,7 +2007,7 @@
       </c>
       <c r="F22" s="2"/>
       <c r="K22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2019,7 +2021,7 @@
         <v>168</v>
       </c>
       <c r="K23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="27">
@@ -2094,7 +2096,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2105,7 +2107,7 @@
         <v>168</v>
       </c>
       <c r="K27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2180,7 +2182,7 @@
       </c>
       <c r="F30" s="2"/>
       <c r="K30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2191,7 +2193,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="K31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="27">
@@ -2264,7 +2266,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2272,7 +2274,7 @@
       <c r="B35" s="2"/>
       <c r="F35" s="2"/>
       <c r="K35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2347,7 +2349,7 @@
       </c>
       <c r="F38" s="2"/>
       <c r="K38" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2358,7 +2360,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="K39" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2527,7 +2529,7 @@
       </c>
       <c r="G48" s="4"/>
       <c r="K48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2544,7 +2546,7 @@
       </c>
       <c r="F49" s="2"/>
       <c r="K49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2558,7 +2560,7 @@
         <v>168</v>
       </c>
       <c r="K50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2717,7 +2719,7 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2734,7 +2736,7 @@
       </c>
       <c r="F59" s="2"/>
       <c r="K59" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2748,7 +2750,7 @@
         <v>168</v>
       </c>
       <c r="K60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2767,7 +2769,7 @@
         <v>78</v>
       </c>
       <c r="K61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="27">
@@ -2781,7 +2783,7 @@
         <v>187</v>
       </c>
       <c r="K62" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -2795,7 +2797,7 @@
         <v>168</v>
       </c>
       <c r="K63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -2814,7 +2816,7 @@
         <v>78</v>
       </c>
       <c r="K64" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="27">
@@ -2828,7 +2830,7 @@
         <v>187</v>
       </c>
       <c r="K65" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -2842,7 +2844,7 @@
         <v>168</v>
       </c>
       <c r="K66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -2861,7 +2863,7 @@
         <v>78</v>
       </c>
       <c r="K67" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="27">
@@ -2875,7 +2877,7 @@
         <v>187</v>
       </c>
       <c r="K68" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -2889,7 +2891,7 @@
         <v>168</v>
       </c>
       <c r="K69" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -2908,7 +2910,7 @@
         <v>78</v>
       </c>
       <c r="K70" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="27">
@@ -2922,7 +2924,7 @@
         <v>187</v>
       </c>
       <c r="K71" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -2936,7 +2938,7 @@
         <v>168</v>
       </c>
       <c r="K72" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -2955,7 +2957,7 @@
         <v>78</v>
       </c>
       <c r="K73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="27">
@@ -2969,7 +2971,7 @@
         <v>187</v>
       </c>
       <c r="K74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -2983,7 +2985,7 @@
         <v>168</v>
       </c>
       <c r="K75" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -3152,7 +3154,7 @@
       <c r="F82" s="2"/>
       <c r="G82" s="4"/>
       <c r="K82" s="7" t="s">
-        <v>195</v>
+        <v>248</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="27">
@@ -3224,7 +3226,7 @@
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D87" s="13" t="s">
         <v>4</v>
@@ -3234,17 +3236,17 @@
       <c r="G87" s="4"/>
       <c r="I87" s="9"/>
       <c r="J87" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K87" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D88" s="13" t="s">
         <v>4</v>
@@ -3254,17 +3256,17 @@
       <c r="G88" s="4"/>
       <c r="I88" s="9"/>
       <c r="J88" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K88" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D89" s="13" t="s">
         <v>4</v>
@@ -3274,7 +3276,7 @@
       <c r="G89" s="4"/>
       <c r="I89" s="9"/>
       <c r="J89" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K89" t="s">
         <v>247</v>
@@ -3284,20 +3286,20 @@
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D90" s="13" t="s">
         <v>240</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>241</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="4"/>
       <c r="I90" s="9"/>
       <c r="J90" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K90" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -3340,7 +3342,7 @@
         <v>193</v>
       </c>
       <c r="K92" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="27">
@@ -3396,7 +3398,7 @@
         <v>165</v>
       </c>
       <c r="K95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="11:11">

</xml_diff>